<commit_message>
feat: Add Export to Excel functionality for Dashboard and Groups
- Implemented ExportToExcelButton component to export dashboard summary and tests summary to Excel.
- Added functionality to sanitize sheet names and format file names with dates.
- Created Groups page with group management features including create, edit, and delete groups.
- Integrated loading state for fetching groups from the API.
</commit_message>
<xml_diff>
--- a/public/sample-users.xlsx
+++ b/public/sample-users.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>email</t>
   </si>
@@ -32,9 +32,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>contact</t>
   </si>
   <si>
@@ -44,19 +41,37 @@
     <t>Onkar Nagarkar</t>
   </si>
   <si>
-    <t>onkarn@techcryptors.com</t>
-  </si>
-  <si>
-    <t>doctor</t>
-  </si>
-  <si>
     <t>Akanksha Indap</t>
   </si>
   <si>
-    <t>akankshai@techcryptors.com</t>
-  </si>
-  <si>
-    <t>physician</t>
+    <t>aid.techcryptors@gmail.com</t>
+  </si>
+  <si>
+    <t>it.techcryptors@gmail.com</t>
+  </si>
+  <si>
+    <t>speciality</t>
+  </si>
+  <si>
+    <t>oncology</t>
+  </si>
+  <si>
+    <t>sports-medicine</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Maharastra</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Raigad</t>
   </si>
 </sst>
 </file>
@@ -392,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,9 +418,9 @@
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -414,15 +429,21 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -431,18 +452,24 @@
         <v>123456</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>9653384868</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>12345678</v>
@@ -452,6 +479,12 @@
       </c>
       <c r="E3">
         <v>9988776655</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>